<commit_message>
guardando hasta antes de modificar productos
</commit_message>
<xml_diff>
--- a/modelado/modeladoprestashop.xlsx
+++ b/modelado/modeladoprestashop.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\erp2027\modelado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131D0698-0C1D-4DAC-9E35-DEDE2D424A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198E095F-A224-4D90-86A7-DC20B70D3B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
   <si>
     <t>verde</t>
   </si>
@@ -268,13 +268,49 @@
   </si>
   <si>
     <t>camisa</t>
+  </si>
+  <si>
+    <t>product_templates</t>
+  </si>
+  <si>
+    <t>attribute_values</t>
+  </si>
+  <si>
+    <t>product_variants</t>
+  </si>
+  <si>
+    <t>product_variant_attribute_value</t>
+  </si>
+  <si>
+    <r>
+      <t>attribute_groups</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>attributes</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +344,35 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -445,12 +510,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -472,7 +536,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,6 +551,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,54 +861,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="2:15" ht="21">
+      <c r="B1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="C1" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="I1" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15">
+      <c r="B2" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="G2" s="25" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14" t="s">
+    <row r="3" spans="2:15">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1"/>
@@ -856,11 +929,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
+    <row r="4" spans="2:15">
+      <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1"/>
@@ -884,11 +957,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="14">
+    <row r="5" spans="2:15">
+      <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -910,11 +983,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
+    <row r="6" spans="2:15">
+      <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -936,11 +1009,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="33">
+    <row r="7" spans="2:15">
+      <c r="B7" s="31">
         <v>5</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -962,11 +1035,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+    <row r="8" spans="2:15" ht="21">
+      <c r="B8" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="36" t="s">
+        <v>82</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="3" t="s">
@@ -985,15 +1060,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:15">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
       <c r="G9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1004,11 +1079,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" s="3">
         <v>36</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3"/>
@@ -1023,11 +1098,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11" s="3">
         <v>37</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="28" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="3"/>
@@ -1042,49 +1117,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12" s="3">
         <v>38</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>19</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" s="3">
         <v>39</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="28" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>20</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" s="3">
         <v>40</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="28" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="3"/>
@@ -1093,117 +1168,120 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15" s="3">
         <v>41</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="28" t="s">
         <v>81</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="26" t="s">
+    <row r="16" spans="2:15" ht="21">
+      <c r="D16" s="34" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D17" s="6" t="s">
+      <c r="E16" s="36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="4:17">
+      <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="23">
+    <row r="18" spans="4:17">
+      <c r="D18" s="22">
         <v>90</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="23">
         <v>36</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>18</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="16" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="23">
+    <row r="19" spans="4:17">
+      <c r="D19" s="22">
         <v>91</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="23">
         <v>36</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <v>18</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="16" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D20" s="23">
+    <row r="20" spans="4:17">
+      <c r="D20" s="22">
         <v>92</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="23">
         <v>36</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>18</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="16" t="s">
+      <c r="H20" s="9"/>
+      <c r="I20" s="15" t="s">
         <v>45</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D21" s="23">
+    <row r="21" spans="4:17">
+      <c r="D21" s="22">
         <v>93</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="23">
         <v>36</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>18</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="16" t="s">
+      <c r="H21" s="9"/>
+      <c r="I21" s="15" t="s">
         <v>46</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:17">
       <c r="D22" s="3">
         <v>94</v>
       </c>
@@ -1221,7 +1299,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:17">
       <c r="D23" s="3">
         <v>95</v>
       </c>
@@ -1239,7 +1317,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:17">
       <c r="D24" s="3">
         <v>96</v>
       </c>
@@ -1255,7 +1333,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:17">
       <c r="D25" s="3">
         <v>97</v>
       </c>
@@ -1268,106 +1346,110 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D26" s="18">
+    <row r="26" spans="4:17">
+      <c r="D26" s="17">
         <v>98</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="17">
         <v>39</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="8">
         <v>600</v>
       </c>
       <c r="G26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D27" s="9">
+    <row r="27" spans="4:17">
+      <c r="D27" s="8">
         <v>99</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D28" s="9">
+    <row r="28" spans="4:17">
+      <c r="D28" s="8">
         <v>100</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D29" s="20">
+    <row r="29" spans="4:17">
+      <c r="D29" s="19">
         <v>101</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="19">
         <v>41</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="21" t="s">
+      <c r="I29" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D30" s="20">
+    <row r="30" spans="4:17">
+      <c r="D30" s="19">
         <v>102</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="19">
         <v>41</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="21" t="s">
+      <c r="I30" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D31" s="20">
+    <row r="31" spans="4:17">
+      <c r="D31" s="19">
         <v>103</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="19">
         <v>41</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="21" t="s">
+      <c r="I31" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D32" s="20">
+    <row r="32" spans="4:17">
+      <c r="D32" s="19">
         <v>104</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="19">
         <v>41</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="21" t="s">
+      <c r="I32" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H38" s="4" t="s">
+    <row r="38" spans="8:11" ht="21">
+      <c r="H38" s="34" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H39" s="7" t="s">
+      <c r="I38" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="J38" s="36"/>
+    </row>
+    <row r="39" spans="8:11">
+      <c r="H39" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I39" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:11">
       <c r="H40" s="3">
         <v>90</v>
       </c>
@@ -1381,7 +1463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:11">
       <c r="H41" s="3">
         <v>90</v>
       </c>
@@ -1395,7 +1477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:11">
       <c r="H42" s="3">
         <v>91</v>
       </c>
@@ -1409,7 +1491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:11">
       <c r="H43" s="3">
         <v>91</v>
       </c>
@@ -1423,7 +1505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:11">
       <c r="H44" s="3">
         <v>92</v>
       </c>
@@ -1434,7 +1516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:11">
       <c r="H45" s="3">
         <v>92</v>
       </c>
@@ -1445,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:11">
       <c r="H46" s="3">
         <v>93</v>
       </c>
@@ -1456,7 +1538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:11">
       <c r="H47" s="3">
         <v>93</v>
       </c>
@@ -1467,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:11">
       <c r="H48" s="3">
         <v>94</v>
       </c>
@@ -1478,7 +1560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10">
       <c r="H49" s="3">
         <v>95</v>
       </c>
@@ -1489,7 +1571,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10">
       <c r="H50" s="3">
         <v>96</v>
       </c>
@@ -1497,7 +1579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10">
       <c r="H51" s="3">
         <v>97</v>
       </c>
@@ -1505,137 +1587,137 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H52" s="19">
+    <row r="52" spans="2:10">
+      <c r="H52" s="18">
         <v>98</v>
       </c>
-      <c r="I52" s="19">
+      <c r="I52" s="18">
         <v>18</v>
       </c>
       <c r="J52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H53" s="17">
+    <row r="53" spans="2:10">
+      <c r="H53" s="16">
         <v>99</v>
       </c>
-      <c r="I53" s="17">
+      <c r="I53" s="16">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H54" s="17">
+    <row r="54" spans="2:10">
+      <c r="H54" s="16">
         <v>100</v>
       </c>
-      <c r="I54" s="17">
+      <c r="I54" s="16">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="10">
-        <v>1</v>
-      </c>
-      <c r="C55" s="10" t="s">
+    <row r="55" spans="2:10">
+      <c r="B55" s="9">
+        <v>1</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H55" s="22">
+      <c r="H55" s="21">
         <v>101</v>
       </c>
-      <c r="I55" s="22">
+      <c r="I55" s="21">
         <v>1</v>
       </c>
       <c r="J55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="10">
+    <row r="56" spans="2:10">
+      <c r="B56" s="9">
         <v>2</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="H56" s="22">
+      <c r="D56" s="9"/>
+      <c r="H56" s="21">
         <v>102</v>
       </c>
-      <c r="I56" s="22">
+      <c r="I56" s="21">
         <v>2</v>
       </c>
       <c r="J56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="10">
+    <row r="57" spans="2:10">
+      <c r="B57" s="9">
         <v>3</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="10"/>
-      <c r="H57" s="22">
+      <c r="D57" s="9"/>
+      <c r="H57" s="21">
         <v>103</v>
       </c>
-      <c r="I57" s="22">
+      <c r="I57" s="21">
         <v>3</v>
       </c>
       <c r="J57" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10">
       <c r="E58" t="s">
         <v>34</v>
       </c>
       <c r="F58" t="s">
         <v>33</v>
       </c>
-      <c r="H58" s="22">
+      <c r="H58" s="21">
         <v>104</v>
       </c>
-      <c r="I58" s="22">
+      <c r="I58" s="21">
         <v>4</v>
       </c>
       <c r="J58" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="10">
+    <row r="59" spans="2:10">
+      <c r="B59" s="9">
         <v>111</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59" s="9">
         <v>3.99</v>
       </c>
-      <c r="F59" s="10">
+      <c r="F59" s="9">
         <v>3.98</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="10">
+    <row r="60" spans="2:10">
+      <c r="B60" s="9">
         <v>112</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="9">
         <v>3.99</v>
       </c>
-      <c r="F60" s="10">
+      <c r="F60" s="9">
         <v>4.05</v>
       </c>
     </row>
@@ -1653,7 +1735,7 @@
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="6" max="6" width="7.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
@@ -1661,55 +1743,55 @@
     <col min="16" max="16" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="2:16">
+      <c r="B2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="F2" s="34" t="s">
+      <c r="C2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+    </row>
+    <row r="3" spans="2:16">
+      <c r="B3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="35"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P3" s="33"/>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -1744,7 +1826,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1779,7 +1861,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -1814,7 +1896,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -1843,14 +1925,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16">
       <c r="F8" s="3">
         <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="26" t="s">
         <v>77</v>
       </c>
       <c r="I8" s="3">
@@ -1882,7 +1964,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
avance de lista de precios
</commit_message>
<xml_diff>
--- a/modelado/modeladoprestashop.xlsx
+++ b/modelado/modeladoprestashop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\erp2027\modelado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E5B612-AC7B-4A33-9E8A-C7B7DDE44B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F07D929-BCB6-4744-87EC-3FA758573A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="840" windowWidth="23730" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>product_variants</t>
-  </si>
-  <si>
-    <t>product_variant_attribute_value</t>
   </si>
   <si>
     <r>
@@ -304,6 +301,9 @@
       </rPr>
       <t>attributes</t>
     </r>
+  </si>
+  <si>
+    <t>attribute_value_product_variant</t>
   </si>
 </sst>
 </file>
@@ -545,16 +545,16 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -878,16 +878,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="21">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="34" t="s">
+      <c r="C1" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="34" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1036,10 +1036,10 @@
       </c>
     </row>
     <row r="8" spans="2:15" ht="21">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="3"/>
@@ -1179,10 +1179,10 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:15" ht="21">
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="34" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1433,13 +1433,13 @@
       </c>
     </row>
     <row r="38" spans="8:11" ht="21">
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I38" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="J38" s="36"/>
+      <c r="I38" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="J38" s="34"/>
     </row>
     <row r="39" spans="8:11">
       <c r="H39" s="6" t="s">
@@ -1744,19 +1744,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="F2" s="32" t="s">
+      <c r="C2" s="36"/>
+      <c r="F2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="3" spans="2:16">
       <c r="B3" s="25" t="s">
@@ -1786,10 +1786,10 @@
       <c r="L3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="O3" s="33" t="s">
+      <c r="O3" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="33"/>
+      <c r="P3" s="37"/>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" s="3">

</xml_diff>